<commit_message>
[Navigation] - Connection between screens (routes)
</commit_message>
<xml_diff>
--- a/Tutorial #/Navigation Flutter.xlsx
+++ b/Tutorial #/Navigation Flutter.xlsx
@@ -8,25 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\development\flutter_project\Tutorial #\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5BD1CD-A026-4067-976A-ED9A3AF8850A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A7B130-6CFB-48B1-8907-0C859DB7AF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Navigation (Routes)" sheetId="1" r:id="rId1"/>
-    <sheet name="Create new Screen" sheetId="2" r:id="rId2"/>
+    <sheet name="Create new Screen" sheetId="2" r:id="rId1"/>
+    <sheet name="Navigation (Routes)" sheetId="1" r:id="rId2"/>
+    <sheet name="(AppBar) - Back btn" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Navigation (Routes)</t>
     <phoneticPr fontId="3"/>
@@ -43,6 +52,91 @@
   </si>
   <si>
     <t>Create new Screen</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">අපි මෙච්චරකල් වැඩ කලේ එක screen එකක් එක්ක </t>
+  </si>
+  <si>
+    <t xml:space="preserve">අපි අලුත් screen එකටත් Scaffold widget එකක් use කරනවා </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>①</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Scaffold හදාගන්න class එකක් හදනව </t>
+  </si>
+  <si>
+    <t xml:space="preserve">කැමති class එකක් කැමති widget type එකෙන් හදාගන්න පුළුවන් </t>
+  </si>
+  <si>
+    <t xml:space="preserve">අපි මෙතැනදී state එකක් manage කරන්න නැති නිසා </t>
+  </si>
+  <si>
+    <t xml:space="preserve">stateless class එකක් හදාගන්නවා </t>
+  </si>
+  <si>
+    <t xml:space="preserve">second screen එක වැඩ කරන විදිය run කරලා බලමු </t>
+  </si>
+  <si>
+    <t>②</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>③</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">අපිට දැන් ඕනේ මේ home page එකේ තියන btn එක </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">click කලාම second screen එකට move වෙන්න </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ඒකට navigation logic එක ලියමු </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>④</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>RUN</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Back btn design </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">කලින් Navigation set කලාම secound page එකේ back btn එකක් auto set වෙලා display උනා </t>
+  </si>
+  <si>
+    <t xml:space="preserve">අපි ඒ back btn එකේ design එක වෙනස් කරමු </t>
+  </si>
+  <si>
+    <t xml:space="preserve">මේක app bar එකට අදාළ දෙයක් </t>
+  </si>
+  <si>
+    <t xml:space="preserve">මුලින්ම icon එක set කරගමු </t>
+  </si>
+  <si>
+    <t xml:space="preserve">btn එක තාම active නැ onpress method එක තාම දාල නැති නිසා </t>
+  </si>
+  <si>
+    <t xml:space="preserve">icon display වෙනවා හැබැයි තාම btn එක වැඩ කරන්නේ නැ </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>(Navigation set කරපු වෙලාවේ btn වැඩ කළා )</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Move logic set කරමු </t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -50,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +177,25 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF0070C0"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="30"/>
+      <color rgb="FF002060"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -104,10 +217,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,6 +636,764 @@
         <a:xfrm>
           <a:off x="731521" y="18032428"/>
           <a:ext cx="4213860" cy="1924013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>121921</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>214598</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>426721</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>252987</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D403066E-48FE-D123-1E74-A11B6EE8D39F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="792481" y="5350478"/>
+          <a:ext cx="4998720" cy="2507269"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>167641</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>83906</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>106681</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>60335</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AE05EEB-C7F7-9DF1-E483-0170EF1DC95F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6202681" y="8100146"/>
+          <a:ext cx="4632960" cy="5325669"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>186074</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>231750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBE11C69-139F-6A9D-BA69-DEC19B254676}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="883920" y="14785994"/>
+          <a:ext cx="5196840" cy="4160476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>175261</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>29201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>327661</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>327661</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56F38BC5-FC00-9ACB-CDFD-FF864FB23F3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6880861" y="16686521"/>
+          <a:ext cx="3505200" cy="2355860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>214689</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>624841</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>327346</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFD680B7-8475-5D01-01A4-2B112216BDE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6606541" y="14814609"/>
+          <a:ext cx="4076700" cy="1758577"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>205740</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>115570</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{742A6862-2A80-B5AF-D875-7E8C2E559473}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="754380" y="8221980"/>
+          <a:ext cx="4061460" cy="5259070"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>190790</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>66971</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FA8C8B1-3E11-AFA3-6B9B-F7767E185DDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2202180" y="20551430"/>
+          <a:ext cx="3185160" cy="2345061"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>290702</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>117545</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8185B7B2-D377-7432-38E8-3217F8654E78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="883920" y="23943182"/>
+          <a:ext cx="4937760" cy="3530163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>640080</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E388EDA-27A7-7882-6473-109D3AA0BC69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="670560" y="28277820"/>
+          <a:ext cx="4663440" cy="3497580"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>172596</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>64424</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8BDBA62-100A-0D95-C37E-A3033708B46E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6111239" y="28351356"/>
+          <a:ext cx="4682145" cy="3500244"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>121076</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>209362</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1FE2D0D-9B52-316E-4763-F56AE4BBBF10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="975360" y="1553636"/>
+          <a:ext cx="3589020" cy="2557166"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>198120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>176578</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>60617</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{988240FE-BF6F-1AF8-B779-D83E168289C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="845820" y="5334000"/>
+          <a:ext cx="4695238" cy="2742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>454749</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>316018</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{243E01F4-54E0-3B99-0D46-1FA6C621B06C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="777240" y="9105900"/>
+          <a:ext cx="4371429" cy="1695238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>68581</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>267482</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295183</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>312420</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7813D68-E185-CC7D-8E47-60FCB88A6D01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="739141" y="12398522"/>
+          <a:ext cx="4249962" cy="2925298"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>626025</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>79622</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AD24AB2-0D73-66B8-C569-92825A34ED42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="899160" y="16101060"/>
+          <a:ext cx="5761905" cy="3104762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>388620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>348522</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>22078</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BE0C2F5-7897-4FDD-825B-7CD790591CD4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="792480" y="19514820"/>
+          <a:ext cx="4249962" cy="2925298"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>294471</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>269769</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>54706</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10570F6B-1F4C-FBBB-8DA7-8CD7F89E6DBE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5658951" y="19560540"/>
+          <a:ext cx="3998658" cy="2912206"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -788,8 +1667,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E245F6-90FC-4BB4-9466-60DA68FB818D}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -798,47 +1677,192 @@
     <col min="1" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" x14ac:dyDescent="1.1499999999999999">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.8">
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.8">
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.8">
-      <c r="B6" s="1" t="s">
-        <v>3</v>
+    <row r="1" spans="1:1" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E245F6-90FC-4BB4-9466-60DA68FB818D}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
   <cols>
     <col min="1" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="48" x14ac:dyDescent="1.1499999999999999">
+    <row r="1" spans="1:10" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="J13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="A35" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="A48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.8">
+      <c r="D49" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.8">
+      <c r="B57" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="A68" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF1E745-59D1-4300-A5D3-591323983891}">
+  <dimension ref="A1:I38"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
+  <cols>
+    <col min="1" max="16384" width="8.796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="48" x14ac:dyDescent="1.1499999999999999">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.8">
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.8">
+      <c r="I5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.8">
+      <c r="I7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.8">
+      <c r="A12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="A21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="A28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="B29" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="A38" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Navigation] - Routes table
</commit_message>
<xml_diff>
--- a/Tutorial #/Navigation Flutter.xlsx
+++ b/Tutorial #/Navigation Flutter.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\development\flutter_project\Tutorial #\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A7B130-6CFB-48B1-8907-0C859DB7AF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C3FC9C-3849-45D4-9D84-1F553098CE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create new Screen" sheetId="2" r:id="rId1"/>
     <sheet name="Navigation (Routes)" sheetId="1" r:id="rId2"/>
     <sheet name="(AppBar) - Back btn" sheetId="4" r:id="rId3"/>
+    <sheet name="Routes table" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Navigation (Routes)</t>
     <phoneticPr fontId="3"/>
@@ -137,6 +138,35 @@
   </si>
   <si>
     <t xml:space="preserve">Move logic set කරමු </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Routes table</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Routes table වලින් අපිට කියන්න පුළුවන් අපේ තියන screens මොනවද කියලා </t>
+  </si>
+  <si>
+    <t xml:space="preserve">screen එකකට නමක් දීලා එක ඕන තැනක path එක name එකකින් දෙන්න පුළුවන් මේ විදියට </t>
+  </si>
+  <si>
+    <t xml:space="preserve">එකට අපි MaterialApp use කරනවා </t>
+  </si>
+  <si>
+    <t xml:space="preserve">මොකද MaterialApp ඕනෑම page එකකට access කරන්න පුළුවන් නිසා </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'/secound' = screen එකට නමක් දෙන්න පුළුවන් </t>
+  </si>
+  <si>
+    <t xml:space="preserve">අපි සාමන්යෙන් navigate කරන විදිය කලින් ඉගෙනගත්තා </t>
+  </si>
+  <si>
+    <t xml:space="preserve">තව විශේෂ ක්‍රමයක් තමයි නමක් එක්ක push කරන එක </t>
+  </si>
+  <si>
+    <t xml:space="preserve">defined කරපු name use කරලා navigate කරමු </t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1394,6 +1424,187 @@
         <a:xfrm>
           <a:off x="5658951" y="19560540"/>
           <a:ext cx="3998658" cy="2912206"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419101</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>290932</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>601981</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>327179</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B36FC09-2D41-1723-0049-6652282A7BB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="419101" y="3369412"/>
+          <a:ext cx="4876800" cy="3328087"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>375236</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>374845</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC33192E-84B2-1619-259B-4C17049AC142}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="358140" y="7157036"/>
+          <a:ext cx="5471160" cy="2879969"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>22981</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>319435</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2271AA2D-BDA8-3770-6D1D-BADD7D1F6E63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="487680" y="10508101"/>
+          <a:ext cx="3870960" cy="3176814"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>399300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>87017</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96B7E0C2-8392-94C2-7119-5788D44E9BD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4922520" y="10472940"/>
+          <a:ext cx="4030980" cy="3391037"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1799,9 +2010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF1E745-59D1-4300-A5D3-591323983891}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
   <cols>
@@ -1868,6 +2077,72 @@
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{752508AC-3770-458D-A5E2-F3240DAB9000}">
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
+  <cols>
+    <col min="1" max="16384" width="8.796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="J10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.8">
+      <c r="J18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.8">
+      <c r="J20" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="10:10" x14ac:dyDescent="0.8">
+      <c r="J22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Navigation] - Data Sending
</commit_message>
<xml_diff>
--- a/Tutorial #/Navigation Flutter.xlsx
+++ b/Tutorial #/Navigation Flutter.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\development\flutter_project\Tutorial #\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C3FC9C-3849-45D4-9D84-1F553098CE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFD2CE0-09E1-4909-85F5-81A54A3239EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create new Screen" sheetId="2" r:id="rId1"/>
     <sheet name="Navigation (Routes)" sheetId="1" r:id="rId2"/>
     <sheet name="(AppBar) - Back btn" sheetId="4" r:id="rId3"/>
     <sheet name="Routes table" sheetId="5" r:id="rId4"/>
+    <sheet name="Sending data" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Navigation (Routes)</t>
     <phoneticPr fontId="3"/>
@@ -168,6 +169,36 @@
   <si>
     <t xml:space="preserve">defined කරපු name use කරලා navigate කරමු </t>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Screen එකකින් screen එකකට data pass කරන විදිය බලමු </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">යවන්න ඕනේ data එක string එකක් විදියට දෙනවා </t>
+  </si>
+  <si>
+    <t xml:space="preserve">මෙතැනදී error display වෙන්නේ </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Class එක ඇතුලේ constructor එකක් හදාගමු </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic ක්‍රමයක් විදියට class එකේ constructor එකට data pass කරමු </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">value තියාගන්න constructor  එකක් නැති නිසා </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Constructor එකට එන value එක screen එකේ print කරමු </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Sending data</t>
   </si>
 </sst>
 </file>
@@ -1605,6 +1636,231 @@
         <a:xfrm>
           <a:off x="4922520" y="10472940"/>
           <a:ext cx="4030980" cy="3391037"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>151194</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>313537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>556927</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>350521</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1481368-9B39-9A09-533D-B3C4B9361988}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="821754" y="2980537"/>
+          <a:ext cx="5099653" cy="2505864"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>219178</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>188220</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5C79683-5518-DDCC-9C86-81BC5480E029}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="807720" y="7000978"/>
+          <a:ext cx="4937760" cy="2437922"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>144781</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>233493</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>317193</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F892AC02-F444-DEB9-BEF4-7AFF9DD5D0A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="815341" y="9761220"/>
+          <a:ext cx="5453192" cy="6390333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>271817</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>163099</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>256595</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A624F755-7A15-E1B3-1029-56A636292496}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7647977" y="9814560"/>
+          <a:ext cx="3244082" cy="2573075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>206972</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>352154</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>350520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EF23F4D-22B7-96D1-14EA-86A934116CD8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7583132" y="12894674"/>
+          <a:ext cx="3542068" cy="2055766"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2086,9 +2342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{752508AC-3770-458D-A5E2-F3240DAB9000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
   <cols>
@@ -2143,6 +2397,67 @@
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF7F288-167B-4CC7-AF5E-AD92CCE18AC6}">
+  <dimension ref="A1:K23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
+  <cols>
+    <col min="1" max="16384" width="8.796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="A1" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.8">
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.8">
+      <c r="B4" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.8">
+      <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.8">
+      <c r="J8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.8">
+      <c r="K9" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.8">
+      <c r="B15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.8">
+      <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>